<commit_message>
feat: preparacion de insumos inflacion mensual y curvas de interes
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/inflacion_mensual.xlsx
+++ b/prototipo_pcr/inputs/inflacion_mensual.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C24865D5-401C-4D51-9985-C928B8F54B2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7ED9C5-0537-4B2D-AA10-774C1755C487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA226786-C10D-4460-B0E7-2F76D212E3DD}"/>
   </bookViews>
@@ -38,10 +38,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>FECHA</t>
+    <t>fecha</t>
   </si>
   <si>
-    <t>TASA</t>
+    <t>tasa</t>
   </si>
 </sst>
 </file>
@@ -467,7 +467,7 @@
   <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
fix: se ajustan decimales en el vector de inflacion
</commit_message>
<xml_diff>
--- a/prototipo_pcr/inputs/inflacion_mensual.xlsx
+++ b/prototipo_pcr/inputs/inflacion_mensual.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\proyectos_sura\Decenal\Prototipo\prototipo-pcr\prototipo_pcr\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7ED9C5-0537-4B2D-AA10-774C1755C487}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6323EB7-494D-41B2-AFE8-A9A77A5182DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA226786-C10D-4460-B0E7-2F76D212E3DD}"/>
   </bookViews>
@@ -48,7 +48,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-* #,##0.000000_-;\-* #,##0.000000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,8 +72,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -80,6 +91,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF2F75B5"/>
         <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -106,32 +123,35 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Millares" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -464,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5C6D981-B64F-429A-8D0C-0D8F0DDBB7E3}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -482,170 +502,458 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
+        <v>44316</v>
+      </c>
+      <c r="B2" s="3">
+        <v>5.9230000000000003E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>44347</v>
+      </c>
+      <c r="B3" s="3">
+        <v>9.9944999999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>44377</v>
+      </c>
+      <c r="B4" s="3">
+        <v>-4.9140000000000002E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>44408</v>
+      </c>
+      <c r="B5" s="3">
+        <v>3.2499E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>44439</v>
+      </c>
+      <c r="B6" s="3">
+        <v>4.4742000000000002E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>44469</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3.8276E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>44500</v>
+      </c>
+      <c r="B8" s="3">
+        <v>1.3359999999999999E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>44530</v>
+      </c>
+      <c r="B9" s="3">
+        <v>4.9529999999999999E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>44561</v>
+      </c>
+      <c r="B10" s="3">
+        <v>7.2641999999999993E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>44592</v>
+      </c>
+      <c r="B11" s="3">
+        <v>1.6657399999999999E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>44620</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1.63389E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>44651</v>
+      </c>
+      <c r="B13" s="3">
+        <v>9.9585000000000003E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>44681</v>
+      </c>
+      <c r="B14" s="3">
+        <v>1.24689E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>44712</v>
+      </c>
+      <c r="B15" s="3">
+        <v>8.4474000000000007E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>44742</v>
+      </c>
+      <c r="B16" s="3">
+        <v>5.0717999999999996E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>44773</v>
+      </c>
+      <c r="B17" s="3">
+        <v>8.1162999999999999E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>44804</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1.0217799999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>44834</v>
+      </c>
+      <c r="B19" s="3">
+        <v>9.2972000000000003E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>44865</v>
+      </c>
+      <c r="B20" s="3">
+        <v>7.1506E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>44895</v>
+      </c>
+      <c r="B21" s="3">
+        <v>7.7264999999999999E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>44926</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1.2554300000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="2">
+        <v>44957</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1.7821299999999998E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="2">
+        <v>44985</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1.6581600000000002E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2">
+        <v>45016</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1.0540799999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2">
+        <v>45046</v>
+      </c>
+      <c r="B26" s="3">
+        <v>7.8108999999999991E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
+        <v>45077</v>
+      </c>
+      <c r="B27" s="3">
+        <v>4.3124000000000001E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
+        <v>45107</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3.0087000000000004E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
+        <v>45138</v>
+      </c>
+      <c r="B29" s="3">
+        <v>5.0172999999999997E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
+        <v>45169</v>
+      </c>
+      <c r="B30" s="3">
+        <v>6.9863E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
+        <v>45199</v>
+      </c>
+      <c r="B31" s="3">
+        <v>5.3749999999999996E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
+        <v>45230</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2.4712000000000002E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
+        <v>45260</v>
+      </c>
+      <c r="B33" s="3">
+        <v>4.7165000000000002E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
+        <v>45291</v>
+      </c>
+      <c r="B34" s="3">
+        <v>4.5329999999999997E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2">
         <v>45322</v>
       </c>
-      <c r="B2" s="3">
-        <v>9.1999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="B35" s="3">
+        <v>9.1639000000000009E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2">
         <v>45351</v>
       </c>
-      <c r="B3" s="3">
-        <v>1.09E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="B36" s="3">
+        <v>1.0865800000000002E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>45382</v>
       </c>
-      <c r="B4" s="3">
-        <v>7.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="B37" s="3">
+        <v>7.0261999999999998E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>45412</v>
       </c>
-      <c r="B5" s="3">
-        <v>5.8999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="B38" s="3">
+        <v>5.9391000000000001E-3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2">
         <v>45443</v>
       </c>
-      <c r="B6" s="3">
-        <v>4.3E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="B39" s="3">
+        <v>4.2529000000000004E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2">
         <v>45473</v>
       </c>
-      <c r="B7" s="3">
-        <v>3.2000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="B40" s="3">
+        <v>3.2478000000000003E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2">
         <v>45504</v>
       </c>
-      <c r="B8" s="3">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="B41" s="3">
+        <v>1.9940000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>45535</v>
       </c>
-      <c r="B9" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="2">
+      <c r="B42" s="3">
+        <v>1.6800000000000002E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>45565</v>
       </c>
-      <c r="B10" s="3">
-        <v>2.3999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="B43" s="3">
+        <v>2.4221999999999998E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>45596</v>
       </c>
-      <c r="B11" s="3">
-        <v>-1.2999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="B44" s="3">
+        <v>-1.3437E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>45626</v>
       </c>
-      <c r="B12" s="3">
-        <v>2.7000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="B45" s="3">
+        <v>2.7265000000000002E-3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="2">
         <v>45657</v>
       </c>
-      <c r="B13" s="3">
-        <v>4.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="B46" s="3">
+        <v>4.5874999999999996E-3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="2">
         <v>45688</v>
       </c>
-      <c r="B14" s="3">
-        <v>9.4000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="2">
+      <c r="B47" s="3">
+        <v>9.3549000000000011E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="2">
         <v>45716</v>
       </c>
-      <c r="B15" s="3">
-        <v>1.14E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="2">
+      <c r="B48" s="3">
+        <v>1.13808E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="2">
         <v>45747</v>
       </c>
-      <c r="B16" s="3">
-        <v>5.1999999999999998E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="2">
+      <c r="B49" s="3">
+        <v>5.2414000000000002E-3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="2">
         <v>45777</v>
       </c>
-      <c r="B17" s="3">
-        <v>6.6E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2">
+      <c r="B50" s="3">
+        <v>6.6311E-3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="2">
         <v>45808</v>
       </c>
-      <c r="B18" s="3">
-        <v>3.2000000000000002E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2">
+      <c r="B51" s="3">
+        <v>3.2007000000000003E-3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="2">
         <v>45838</v>
       </c>
-      <c r="B19" s="3">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2">
+      <c r="B52" s="3">
+        <v>1.0318E-3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="2">
         <v>45869</v>
       </c>
-      <c r="B20" s="3">
-        <v>2.8E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2">
+      <c r="B53" s="3">
+        <v>2.7624999999999998E-3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="2">
         <v>45900</v>
       </c>
-      <c r="B21" s="3">
-        <v>1.9E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2">
+      <c r="B54" s="3">
+        <v>1.8768000000000001E-3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="2">
         <v>45930</v>
       </c>
-      <c r="B22" s="3">
-        <v>3.2000000000000002E-3</v>
+      <c r="B55" s="3">
+        <v>3.1963000000000004E-3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="2">
+        <v>45961</v>
+      </c>
+      <c r="B56" s="3">
+        <v>1.8418000000000002E-3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="2">
+        <v>45991</v>
+      </c>
+      <c r="B57" s="3">
+        <v>7.1980000000000004E-4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="2">
+        <v>46022</v>
+      </c>
+      <c r="B58" s="3">
+        <v>2.6681000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>